<commit_message>
browser stack firefox browser code added
</commit_message>
<xml_diff>
--- a/src/test/java/resources/config/TestData.xlsx
+++ b/src/test/java/resources/config/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationLearn\TestNG\src\test\java\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java_projects\SeleniumJavaPOC\src\test\java\resources\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CD9177-FFA5-4928-AC33-F1A962ABA456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CE3D71-EF03-46A2-9764-028DFAC6E291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>productName_1</t>
   </si>
   <si>
-    <t>ZARA COAT 3</t>
-  </si>
-  <si>
     <t>confirmMessage_1</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>confirmMessage_6</t>
+  </si>
+  <si>
+    <t>IPHONE 13 PRO</t>
   </si>
 </sst>
 </file>
@@ -187,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -202,17 +202,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,19 +493,19 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="39.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +516,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -534,11 +531,11 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2"/>
@@ -549,11 +546,11 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3"/>
@@ -564,132 +561,132 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="10" t="s">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="B9" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="B10" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="B11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="10" t="s">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="B12" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="B13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="10" t="s">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="B14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="10" t="s">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="B15" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="B16" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="B17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="10" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="B18" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="B19" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>15</v>
+      <c r="B20" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
basetest class code changes
</commit_message>
<xml_diff>
--- a/src/test/java/resources/config/TestData.xlsx
+++ b/src/test/java/resources/config/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java_projects\SeleniumJavaPOC\src\test\java\resources\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C6F09C-EDF6-4822-8F16-E423FC42BF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BBCFFD-025B-4636-B800-EA29870A0C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
   <si>
     <t>Key</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>productName_2</t>
-  </si>
-  <si>
-    <t>ADIDAS ORIGINAL</t>
   </si>
   <si>
     <t>confirmMessage_2</t>
@@ -492,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,7 +579,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -614,12 +611,12 @@
         <v>17</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>14</v>
@@ -627,31 +624,31 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>14</v>
@@ -659,31 +656,31 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>14</v>

</xml_diff>